<commit_message>
Trying to understand the problem
</commit_message>
<xml_diff>
--- a/CH-062 Missing Values.xlsx
+++ b/CH-062 Missing Values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{D494A47E-3168-4E45-A907-D006C73095CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36D489DC-16EF-45D0-AC59-7958F986F48C}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{D494A47E-3168-4E45-A907-D006C73095CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29F91748-3E3A-4B1E-B967-E970443E0497}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="9">
   <si>
     <t>Question Tables</t>
   </si>
@@ -303,10 +303,10 @@
     <xf numFmtId="9" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="6" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="6" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -997,17 +997,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
+      <c r="H1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -1661,8 +1661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{883E9067-84FC-4922-9F1A-B461FB03985D}">
   <dimension ref="A1:U105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1672,24 +1672,24 @@
     <col min="4" max="4" width="13.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.3984375" customWidth="1"/>
     <col min="6" max="6" width="38.59765625" customWidth="1"/>
-    <col min="7" max="7" width="8.3984375" customWidth="1"/>
+    <col min="7" max="7" width="8.69921875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.3984375" customWidth="1"/>
     <col min="9" max="9" width="8" customWidth="1"/>
     <col min="10" max="10" width="13.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
+      <c r="H1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -2310,7 +2310,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="13" t="s">
         <v>8</v>
       </c>
       <c r="H26" s="11">
@@ -2928,7 +2928,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="70" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B70" s="11" cm="1">
         <f t="array" ref="B70:D105">_xlfn.LET(
 _xlpm.c,_xlfn.UNIQUE(C3:C21),
@@ -2946,8 +2946,20 @@
       <c r="D70" s="10">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="71" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H70">
+        <v>44957</v>
+      </c>
+      <c r="I70" t="s">
+        <v>5</v>
+      </c>
+      <c r="J70">
+        <v>0.02</v>
+      </c>
+      <c r="K70">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="71" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B71" s="11">
         <v>44985</v>
       </c>
@@ -2957,8 +2969,20 @@
       <c r="D71" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="72" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H71">
+        <v>44985</v>
+      </c>
+      <c r="I71" t="s">
+        <v>5</v>
+      </c>
+      <c r="J71">
+        <v>0.04</v>
+      </c>
+      <c r="K71">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="72" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B72" s="11">
         <v>45016</v>
       </c>
@@ -2968,8 +2992,49 @@
       <c r="D72" s="10">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="73" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F72" cm="1">
+        <f t="array" ref="F72">_xlfn.XMATCH(B72&amp;C72,B70:B105&amp;C70:C105)</f>
+        <v>3</v>
+      </c>
+      <c r="H72">
+        <v>45016</v>
+      </c>
+      <c r="I72" t="s">
+        <v>5</v>
+      </c>
+      <c r="J72">
+        <v>0.08</v>
+      </c>
+      <c r="K72" t="b">
+        <f>ISBLANK(J72)</f>
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <f>J71</f>
+        <v>0.04</v>
+      </c>
+      <c r="M72">
+        <f>_xlfn.XLOOKUP(L72+0.00001,$J$70:$J$81,J70:J81,,1)</f>
+        <v>0.08</v>
+      </c>
+      <c r="N72">
+        <f>_xlfn.XMATCH(M72,$J$70:$J$81)</f>
+        <v>3</v>
+      </c>
+      <c r="O72">
+        <f>_xlfn.XMATCH(L72,J70:J81)</f>
+        <v>2</v>
+      </c>
+      <c r="P72">
+        <f>N72-O72</f>
+        <v>1</v>
+      </c>
+      <c r="Q72">
+        <f>(M72-L72)/P72</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="73" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B73" s="11">
         <v>45046</v>
       </c>
@@ -2979,8 +3044,45 @@
       <c r="D73" s="12" t="str">
         <v/>
       </c>
-    </row>
-    <row r="74" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H73">
+        <v>45046</v>
+      </c>
+      <c r="I73" t="s">
+        <v>5</v>
+      </c>
+      <c r="J73">
+        <v>0.12</v>
+      </c>
+      <c r="K73" t="b">
+        <f>ISBLANK(J73)</f>
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <f>J72</f>
+        <v>0.08</v>
+      </c>
+      <c r="M73">
+        <f>_xlfn.XLOOKUP(J72+0.00001,$J$70:$J$81,J70:J81,,1)</f>
+        <v>0.12</v>
+      </c>
+      <c r="N73">
+        <f>_xlfn.XMATCH(M73,$J$70:$J$81)</f>
+        <v>4</v>
+      </c>
+      <c r="O73">
+        <f>_xlfn.XMATCH(L73,J70:J82)</f>
+        <v>3</v>
+      </c>
+      <c r="P73">
+        <f>N73-O73</f>
+        <v>1</v>
+      </c>
+      <c r="Q73">
+        <f>(M73-L73)/P73</f>
+        <v>3.9999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B74" s="11">
         <v>45077</v>
       </c>
@@ -2990,8 +3092,20 @@
       <c r="D74" s="12" t="str">
         <v/>
       </c>
-    </row>
-    <row r="75" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H74">
+        <v>45077</v>
+      </c>
+      <c r="I74" t="s">
+        <v>5</v>
+      </c>
+      <c r="J74">
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="K74">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="75" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B75" s="11">
         <v>45107</v>
       </c>
@@ -3001,8 +3115,20 @@
       <c r="D75" s="12" t="str">
         <v/>
       </c>
-    </row>
-    <row r="76" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H75">
+        <v>45107</v>
+      </c>
+      <c r="I75" t="s">
+        <v>5</v>
+      </c>
+      <c r="J75">
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="K75">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="76" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B76" s="11">
         <v>45138</v>
       </c>
@@ -3012,8 +3138,35 @@
       <c r="D76" s="10">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="77" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H76">
+        <v>45138</v>
+      </c>
+      <c r="I76" t="s">
+        <v>5</v>
+      </c>
+      <c r="J76">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="K76" t="b">
+        <v>0</v>
+      </c>
+      <c r="L76">
+        <f>_xlfn.XLOOKUP(J75+0.0001,J70:J81,J70:J81,,1)</f>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="M76">
+        <v>0.21</v>
+      </c>
+      <c r="N76">
+        <f>_xlfn.XMATCH(L76,J76:J81)</f>
+        <v>1</v>
+      </c>
+      <c r="Q76">
+        <f>(L76-M76)/N76</f>
+        <v>1.5000000000000013E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B77" s="11">
         <v>45169</v>
       </c>
@@ -3023,8 +3176,20 @@
       <c r="D77" s="12" t="str">
         <v/>
       </c>
-    </row>
-    <row r="78" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H77">
+        <v>45169</v>
+      </c>
+      <c r="I77" t="s">
+        <v>5</v>
+      </c>
+      <c r="J77">
+        <v>0.24000000000000002</v>
+      </c>
+      <c r="K77">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="78" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B78" s="11">
         <v>45199</v>
       </c>
@@ -3034,8 +3199,33 @@
       <c r="D78" s="10">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="79" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H78">
+        <v>45199</v>
+      </c>
+      <c r="I78" t="s">
+        <v>5</v>
+      </c>
+      <c r="J78">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L78">
+        <f>_xlfn.XLOOKUP(J77+0.000001,J78:J81,J78:J81,,1)</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M78">
+        <f>J77</f>
+        <v>0.24000000000000002</v>
+      </c>
+      <c r="N78">
+        <f>_xlfn.XMATCH(L78,J78:J81)</f>
+        <v>1</v>
+      </c>
+      <c r="Q78">
+        <f>(L78-M78)/N78</f>
+        <v>4.9999999999999961E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B79" s="11">
         <v>45230</v>
       </c>
@@ -3045,8 +3235,17 @@
       <c r="D79" s="12" t="str">
         <v/>
       </c>
-    </row>
-    <row r="80" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H79">
+        <v>45230</v>
+      </c>
+      <c r="I79" t="s">
+        <v>5</v>
+      </c>
+      <c r="J79">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="80" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B80" s="11">
         <v>45260</v>
       </c>
@@ -3056,8 +3255,17 @@
       <c r="D80" s="12" t="str">
         <v/>
       </c>
-    </row>
-    <row r="81" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H80">
+        <v>45260</v>
+      </c>
+      <c r="I80" t="s">
+        <v>5</v>
+      </c>
+      <c r="J80">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="81" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B81" s="11">
         <v>45291</v>
       </c>
@@ -3067,8 +3275,17 @@
       <c r="D81" s="10">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="82" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H81">
+        <v>45291</v>
+      </c>
+      <c r="I81" t="s">
+        <v>5</v>
+      </c>
+      <c r="J81">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="82" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B82" s="11">
         <v>44957</v>
       </c>
@@ -3079,7 +3296,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="83" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B83" s="11">
         <v>44985</v>
       </c>
@@ -3090,7 +3307,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="84" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B84" s="11">
         <v>45016</v>
       </c>
@@ -3101,7 +3318,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B85" s="11">
         <v>45046</v>
       </c>
@@ -3112,7 +3329,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B86" s="11">
         <v>45077</v>
       </c>
@@ -3123,7 +3340,7 @@
         <v>0.16000000000000003</v>
       </c>
     </row>
-    <row r="87" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B87" s="11">
         <v>45107</v>
       </c>
@@ -3134,7 +3351,7 @@
         <v>0.21000000000000002</v>
       </c>
     </row>
-    <row r="88" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B88" s="11">
         <v>45138</v>
       </c>
@@ -3145,7 +3362,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B89" s="11">
         <v>45169</v>
       </c>
@@ -3156,7 +3373,7 @@
         <v>0.24000000000000002</v>
       </c>
     </row>
-    <row r="90" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B90" s="11">
         <v>45199</v>
       </c>
@@ -3167,7 +3384,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B91" s="11">
         <v>45230</v>
       </c>
@@ -3178,7 +3395,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B92" s="11">
         <v>45260</v>
       </c>
@@ -3189,7 +3406,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B93" s="11">
         <v>45291</v>
       </c>
@@ -3200,7 +3417,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="94" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B94" s="11">
         <v>44957</v>
       </c>
@@ -3211,7 +3428,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="95" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B95" s="11">
         <v>44985</v>
       </c>
@@ -3222,7 +3439,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B96" s="11">
         <v>45016</v>
       </c>

</xml_diff>

<commit_message>
Nearing the end. Single function work going on.
</commit_message>
<xml_diff>
--- a/CH-062 Missing Values.xlsx
+++ b/CH-062 Missing Values.xlsx
@@ -1,24 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{D494A47E-3168-4E45-A907-D006C73095CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29F91748-3E3A-4B1E-B967-E970443E0497}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D28567-4DCA-43BE-8420-4ABFA642075B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Experiment" sheetId="3" r:id="rId3"/>
+    <sheet name="SingleFunction" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$G$2:$I$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$G$2:$I$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">SingleFunction!$G$2:$I$10</definedName>
+    <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="10">
   <si>
     <t>Question Tables</t>
   </si>
@@ -91,22 +95,25 @@
   <si>
     <t>CH-054 Solution</t>
   </si>
+  <si>
+    <t/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Century Gothic"/>
+      <name val="Consolas"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Century Gothic"/>
+      <name val="Consolas"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -120,7 +127,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Century Gothic"/>
+      <name val="Consolas"/>
       <family val="1"/>
       <scheme val="minor"/>
     </font>
@@ -151,8 +158,23 @@
       <name val="Aptos Mono"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +196,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF938CBE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -267,11 +295,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -304,13 +334,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="6" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Intro_Hd" xfId="3" xr:uid="{464B17D7-087D-4543-A532-640BE73C2EE2}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{92DAC45E-EA74-418C-9EB0-1EB872499779}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -361,8 +397,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3314700" y="554990"/>
-          <a:ext cx="4552316" cy="4074795"/>
+          <a:off x="3314700" y="558800"/>
+          <a:ext cx="4556126" cy="4029075"/>
           <a:chOff x="4132802" y="1860550"/>
           <a:chExt cx="3791314" cy="2737366"/>
         </a:xfrm>
@@ -733,9 +769,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Wisp">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Biegert_Plum">
   <a:themeElements>
-    <a:clrScheme name="Wisp">
+    <a:clrScheme name="BIegert Plum Scheme">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -743,153 +779,129 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="766F54"/>
+        <a:srgbClr val="4E3B30"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E3EACF"/>
+        <a:srgbClr val="FBEEC9"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="A53010"/>
+        <a:srgbClr val="803975"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="DE7E18"/>
+        <a:srgbClr val="58204D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9F8351"/>
+        <a:srgbClr val="B44A5E"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="728653"/>
+        <a:srgbClr val="D2666D"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="92AA4C"/>
+        <a:srgbClr val="FAB395"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="6AAC91"/>
+        <a:srgbClr val="F2D48E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="FB4A18"/>
+        <a:srgbClr val="00B0F0"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="FB9318"/>
+        <a:srgbClr val="00B050"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Wisp">
+    <a:fontScheme name="Biegert Plum Fonts">
       <a:majorFont>
-        <a:latin typeface="Century Gothic" panose="020B0502020202020204"/>
+        <a:latin typeface="Aptos Mono"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="メイリオ"/>
-        <a:font script="Hang" typeface="HY중고딕"/>
-        <a:font script="Hans" typeface="幼圆"/>
-        <a:font script="Hant" typeface="微軟正黑體"/>
-        <a:font script="Arab" typeface="Tahoma"/>
-        <a:font script="Hebr" typeface="Gisha"/>
-        <a:font script="Thai" typeface="DilleniaUPC"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Tahoma"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Century Gothic" panose="020B0502020202020204"/>
+        <a:latin typeface="Consolas"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="メイリオ"/>
-        <a:font script="Hang" typeface="HY중고딕"/>
-        <a:font script="Hans" typeface="幼圆"/>
-        <a:font script="Hant" typeface="微軟正黑體"/>
-        <a:font script="Arab" typeface="Tahoma"/>
-        <a:font script="Hebr" typeface="Gisha"/>
-        <a:font script="Thai" typeface="DilleniaUPC"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Tahoma"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Wisp">
+    <a:fmtScheme name="Glossy">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="70000"/>
-            <a:lumMod val="104000"/>
-          </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="96000"/>
-                <a:lumMod val="104000"/>
+                <a:tint val="62000"/>
+                <a:satMod val="180000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="65000">
+              <a:schemeClr val="phClr">
+                <a:tint val="32000"/>
+                <a:satMod val="250000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="98000"/>
-                <a:lumMod val="94000"/>
+                <a:tint val="23000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="15000"/>
+                <a:satMod val="180000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:shade val="45000"/>
+                <a:satMod val="170000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="70000">
+              <a:schemeClr val="phClr">
+                <a:tint val="99000"/>
+                <a:shade val="65000"/>
+                <a:satMod val="155000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="95500"/>
+                <a:shade val="100000"/>
+                <a:satMod val="155000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="rnd" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="90000"/>
+              <a:tint val="95000"/>
+              <a:shade val="95000"/>
+              <a:satMod val="120000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="15875" cap="rnd" cmpd="sng" algn="ctr">
+        <a:ln w="55000" cap="flat" cmpd="thickThin" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="phClr"/>
+            <a:schemeClr val="phClr">
+              <a:tint val="90000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+        <a:ln w="50800" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -898,13 +910,10 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="50800" dist="38100" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="25000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -913,54 +922,73 @@
           <a:effectLst>
             <a:outerShdw blurRad="50800" dist="38100" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="60000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="63500" dist="38100" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="45000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="glow" dir="t">
+              <a:rot lat="0" lon="0" rev="6360000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d contourW="1000" prstMaterial="flat">
+            <a:bevelT w="95250" h="101600"/>
+            <a:contourClr>
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:contourClr>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="90000"/>
-                <a:lumMod val="120000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="98000"/>
+                <a:shade val="63000"/>
                 <a:satMod val="120000"/>
-                <a:lumMod val="98000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="90000"/>
-                <a:satMod val="92000"/>
-                <a:lumMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="98000"/>
-                <a:satMod val="120000"/>
-                <a:lumMod val="98000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="100000" b="100000"/>
-          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -969,10 +997,40 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Wisp" id="{7CB32D59-10C0-40DD-B7BD-2E94284A981C}" vid="{24B1A44C-C006-48B2-A4D7-E5549B3D8CD4}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
+</file>
+
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="937" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{C267957B-A9F2-4089-9F7C-2EB4C8BA672A}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -983,33 +1041,33 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
     <col min="2" max="3" width="12.3984375" customWidth="1"/>
-    <col min="4" max="4" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.19921875" customWidth="1"/>
     <col min="5" max="5" width="15.3984375" customWidth="1"/>
     <col min="6" max="6" width="38.59765625" customWidth="1"/>
     <col min="7" max="7" width="8.3984375" customWidth="1"/>
     <col min="8" max="8" width="15.3984375" customWidth="1"/>
     <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-    </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+    </row>
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="9" t="s">
         <v>2</v>
@@ -1661,37 +1719,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{883E9067-84FC-4922-9F1A-B461FB03985D}">
   <dimension ref="A1:U105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J69" sqref="J69"/>
+    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
     <col min="2" max="3" width="12.3984375" customWidth="1"/>
-    <col min="4" max="4" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.19921875" customWidth="1"/>
     <col min="5" max="5" width="15.3984375" customWidth="1"/>
     <col min="6" max="6" width="38.59765625" customWidth="1"/>
-    <col min="7" max="7" width="8.69921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.69921875" customWidth="1"/>
     <col min="8" max="8" width="15.3984375" customWidth="1"/>
     <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-    </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+    </row>
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="9" t="s">
         <v>2</v>
@@ -1734,10 +1792,10 @@
       </c>
       <c r="L3" s="1" t="b" cm="1">
         <f t="array" ref="L3:M38">H3:I38=B29:C64</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:21" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1761,10 +1819,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L4" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:21" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1788,10 +1846,10 @@
         <v>0.08</v>
       </c>
       <c r="L5" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1815,10 +1873,10 @@
         <v>0.12</v>
       </c>
       <c r="L6" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:21" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1842,10 +1900,10 @@
         <v>0.15999999999999998</v>
       </c>
       <c r="L7" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1870,10 +1928,10 @@
         <v>0.19999999999999996</v>
       </c>
       <c r="L8" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1897,10 +1955,10 @@
         <v>0.24</v>
       </c>
       <c r="L9" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1924,10 +1982,10 @@
         <v>0.25</v>
       </c>
       <c r="L10" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1951,10 +2009,10 @@
         <v>0.26</v>
       </c>
       <c r="L11" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11"/>
       <c r="T11"/>
@@ -1983,10 +2041,10 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R12" s="1"/>
     </row>
@@ -2013,10 +2071,10 @@
         <v>0.31999999999999995</v>
       </c>
       <c r="L13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R13" s="1"/>
     </row>
@@ -2042,10 +2100,10 @@
         <v>0.35</v>
       </c>
       <c r="L14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
@@ -2069,10 +2127,10 @@
         <v>0.02</v>
       </c>
       <c r="L15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
@@ -2096,10 +2154,10 @@
         <v>0.04</v>
       </c>
       <c r="L16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -2123,10 +2181,10 @@
         <v>8.0000000000000016E-2</v>
       </c>
       <c r="L17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -2150,10 +2208,10 @@
         <v>0.12000000000000002</v>
       </c>
       <c r="L18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -2177,10 +2235,10 @@
         <v>0.16000000000000003</v>
       </c>
       <c r="L19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -2204,10 +2262,10 @@
         <v>0.21000000000000002</v>
       </c>
       <c r="L20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -2231,10 +2289,10 @@
         <v>0.22500000000000003</v>
       </c>
       <c r="L21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -2249,10 +2307,10 @@
         <v>0.24000000000000002</v>
       </c>
       <c r="L22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -2267,10 +2325,10 @@
         <v>0.29000000000000004</v>
       </c>
       <c r="L23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -2285,10 +2343,10 @@
         <v>0.34</v>
       </c>
       <c r="L24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -2303,10 +2361,10 @@
         <v>0.39</v>
       </c>
       <c r="L25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -2323,10 +2381,10 @@
         <v>0.44</v>
       </c>
       <c r="L26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
@@ -2341,10 +2399,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -2359,32 +2417,28 @@
         <v>0.14500000000000002</v>
       </c>
       <c r="L28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="11" cm="1">
-        <f t="array" ref="B29:D64">_xlfn.LET(
+        <f t="array" ref="B29:B64">_xlfn.LET(
 _xlpm.c,_xlfn.UNIQUE(C3:C21),
 _xlpm.q,_xlfn.REDUCE("",_xlpm.c,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.LET(_xlpm.t,_xlfn._xlws.FILTER(B3:C21,C3:C21=_xlpm.v),_xlpm.mx,MAX(_xlfn.TAKE(_xlpm.t,,1)),_xlpm.mn,MIN(_xlfn.TAKE(_xlpm.t,,1)),_xlfn.VSTACK(_xlpm.a,_xlfn.LET(_xlpm.zz,_xlfn.UNIQUE(EOMONTH(_xlfn.SEQUENCE(_xlpm.mx-_xlpm.mn+1,1,_xlpm.mn),0)),_xlpm.yy,_xlfn.MAKEARRAY(LEN(_xlpm.zz),1,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,_xlpm.v)),_xlfn.HSTACK(_xlpm.zz,_xlpm.yy)))))),
 _xlpm._q,_xlfn.DROP(_xlpm.q,1),
 _xlpm.r,_xlfn.BYROW(_xlpm._q,_xlfn.LAMBDA(_xlpm.r,_xlfn.TEXTJOIN("",TRUE,_xlpm.r))),
 _xlpm.mm,_xlfn.XLOOKUP(_xlpm.r,B3:B21&amp;C3:C21,D3:D21,""),
 _xlpm.vv,_xlfn.DROP(_xlfn.REDUCE("",_xlpm.mm,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,IF(_xlpm.v="",_xlfn.TAKE(_xlpm.a,-1),_xlpm.v)))),1),
-_xlfn.HSTACK(_xlpm._q,_xlpm.vv)
+_xlpm.vv
 )</f>
-        <v>44957</v>
-      </c>
-      <c r="C29" s="8" t="str">
-        <v>A</v>
-      </c>
-      <c r="D29" s="10">
         <v>0.05</v>
       </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="10"/>
       <c r="H29" s="11">
         <v>45016</v>
       </c>
@@ -2395,23 +2449,19 @@
         <v>0.22000000000000003</v>
       </c>
       <c r="L29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="11">
-        <v>44985</v>
-      </c>
-      <c r="C30" s="8" t="str">
-        <v>A</v>
-      </c>
-      <c r="D30" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="10"/>
       <c r="H30" s="11">
         <v>45046</v>
       </c>
@@ -2422,23 +2472,19 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="11">
-        <v>45016</v>
-      </c>
-      <c r="C31" s="8" t="str">
-        <v>A</v>
-      </c>
-      <c r="D31" s="10">
         <v>0.08</v>
       </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="10"/>
       <c r="H31" s="11">
         <v>45077</v>
       </c>
@@ -2449,22 +2495,18 @@
         <v>0.34</v>
       </c>
       <c r="L31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="11">
-        <v>45046</v>
-      </c>
-      <c r="C32" s="8" t="str">
-        <v>A</v>
-      </c>
-      <c r="D32" s="12">
         <v>0.08</v>
       </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="12"/>
       <c r="H32" s="11">
         <v>45107</v>
       </c>
@@ -2475,23 +2517,19 @@
         <v>0.39</v>
       </c>
       <c r="L32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="11">
-        <v>45077</v>
-      </c>
-      <c r="C33" s="8" t="str">
-        <v>A</v>
-      </c>
-      <c r="D33" s="12">
         <v>0.08</v>
       </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="12"/>
       <c r="H33" s="11">
         <v>45138</v>
       </c>
@@ -2502,22 +2540,18 @@
         <v>0.44</v>
       </c>
       <c r="L33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="11">
-        <v>45107</v>
-      </c>
-      <c r="C34" s="8" t="str">
-        <v>A</v>
-      </c>
-      <c r="D34" s="12">
         <v>0.08</v>
       </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="12"/>
       <c r="H34" s="11">
         <v>45169</v>
       </c>
@@ -2528,23 +2562,19 @@
         <v>0.52</v>
       </c>
       <c r="L34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="11">
-        <v>45138</v>
-      </c>
-      <c r="C35" s="8" t="str">
-        <v>A</v>
-      </c>
-      <c r="D35" s="10">
         <v>0.24</v>
       </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="10"/>
       <c r="H35" s="11">
         <v>45199</v>
       </c>
@@ -2555,23 +2585,19 @@
         <v>0.6</v>
       </c>
       <c r="L35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="11">
-        <v>45169</v>
-      </c>
-      <c r="C36" s="8" t="str">
-        <v>A</v>
-      </c>
-      <c r="D36" s="12">
         <v>0.24</v>
       </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="12"/>
       <c r="H36" s="11">
         <v>45230</v>
       </c>
@@ -2582,23 +2608,19 @@
         <v>0.65999999999999992</v>
       </c>
       <c r="L36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="11">
-        <v>45199</v>
-      </c>
-      <c r="C37" s="8" t="str">
-        <v>A</v>
-      </c>
-      <c r="D37" s="10">
         <v>0.26</v>
       </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="10"/>
       <c r="H37" s="11">
         <v>45260</v>
       </c>
@@ -2609,23 +2631,19 @@
         <v>0.72</v>
       </c>
       <c r="L37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="11">
-        <v>45230</v>
-      </c>
-      <c r="C38" s="8" t="str">
-        <v>A</v>
-      </c>
-      <c r="D38" s="12">
         <v>0.26</v>
       </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="12"/>
       <c r="H38" s="11">
         <v>45291</v>
       </c>
@@ -2636,297 +2654,193 @@
         <v>0.73</v>
       </c>
       <c r="L38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B39" s="11">
-        <v>45260</v>
-      </c>
-      <c r="C39" s="8" t="str">
-        <v>A</v>
-      </c>
-      <c r="D39" s="12">
         <v>0.26</v>
       </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="12"/>
     </row>
     <row r="40" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B40" s="11">
-        <v>45291</v>
-      </c>
-      <c r="C40" s="8" t="str">
-        <v>A</v>
-      </c>
-      <c r="D40" s="10">
         <v>0.35</v>
       </c>
+      <c r="C40" s="8"/>
+      <c r="D40" s="10"/>
     </row>
     <row r="41" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B41" s="11">
-        <v>44957</v>
-      </c>
-      <c r="C41" s="8" t="str">
-        <v>B</v>
-      </c>
-      <c r="D41" s="10">
         <v>0.02</v>
       </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="10"/>
     </row>
     <row r="42" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B42" s="11">
-        <v>44985</v>
-      </c>
-      <c r="C42" s="8" t="str">
-        <v>B</v>
-      </c>
-      <c r="D42" s="10">
         <v>0.04</v>
       </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B43" s="11">
-        <v>45016</v>
-      </c>
-      <c r="C43" s="8" t="str">
-        <v>B</v>
-      </c>
-      <c r="D43" s="12">
         <v>0.04</v>
       </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="12"/>
     </row>
     <row r="44" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B44" s="11">
-        <v>45046</v>
-      </c>
-      <c r="C44" s="8" t="str">
-        <v>B</v>
-      </c>
-      <c r="D44" s="12">
         <v>0.04</v>
       </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="12"/>
     </row>
     <row r="45" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B45" s="11">
-        <v>45077</v>
-      </c>
-      <c r="C45" s="8" t="str">
-        <v>B</v>
-      </c>
-      <c r="D45" s="10">
         <v>0.16000000000000003</v>
       </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="10"/>
     </row>
     <row r="46" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B46" s="11">
-        <v>45107</v>
-      </c>
-      <c r="C46" s="8" t="str">
-        <v>B</v>
-      </c>
-      <c r="D46" s="10">
         <v>0.21000000000000002</v>
       </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="10"/>
     </row>
     <row r="47" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B47" s="11">
-        <v>45138</v>
-      </c>
-      <c r="C47" s="8" t="str">
-        <v>B</v>
-      </c>
-      <c r="D47" s="12">
         <v>0.21000000000000002</v>
       </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="12"/>
     </row>
     <row r="48" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B48" s="11">
-        <v>45169</v>
-      </c>
-      <c r="C48" s="8" t="str">
-        <v>B</v>
-      </c>
-      <c r="D48" s="10">
         <v>0.24000000000000002</v>
       </c>
+      <c r="C48" s="8"/>
+      <c r="D48" s="10"/>
     </row>
     <row r="49" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B49" s="11">
-        <v>45199</v>
-      </c>
-      <c r="C49" s="8" t="str">
-        <v>B</v>
-      </c>
-      <c r="D49" s="12">
         <v>0.24000000000000002</v>
       </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="12"/>
     </row>
     <row r="50" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B50" s="11">
-        <v>45230</v>
-      </c>
-      <c r="C50" s="8" t="str">
-        <v>B</v>
-      </c>
-      <c r="D50" s="12">
         <v>0.24000000000000002</v>
       </c>
+      <c r="C50" s="8"/>
+      <c r="D50" s="12"/>
     </row>
     <row r="51" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B51" s="11">
-        <v>45260</v>
-      </c>
-      <c r="C51" s="8" t="str">
-        <v>B</v>
-      </c>
-      <c r="D51" s="12">
         <v>0.24000000000000002</v>
       </c>
+      <c r="C51" s="8"/>
+      <c r="D51" s="12"/>
     </row>
     <row r="52" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B52" s="11">
-        <v>45291</v>
-      </c>
-      <c r="C52" s="8" t="str">
-        <v>B</v>
-      </c>
-      <c r="D52" s="10">
         <v>0.44</v>
       </c>
+      <c r="C52" s="8"/>
+      <c r="D52" s="10"/>
     </row>
     <row r="53" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B53" s="11">
-        <v>44957</v>
-      </c>
-      <c r="C53" s="8" t="str">
-        <v>C</v>
-      </c>
-      <c r="D53" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
+      <c r="C53" s="8"/>
+      <c r="D53" s="10"/>
     </row>
     <row r="54" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B54" s="11">
-        <v>44985</v>
-      </c>
-      <c r="C54" s="8" t="str">
-        <v>C</v>
-      </c>
-      <c r="D54" s="12">
         <v>7.0000000000000007E-2</v>
       </c>
+      <c r="C54" s="8"/>
+      <c r="D54" s="12"/>
     </row>
     <row r="55" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B55" s="11">
-        <v>45016</v>
-      </c>
-      <c r="C55" s="8" t="str">
-        <v>C</v>
-      </c>
-      <c r="D55" s="10">
         <v>0.22000000000000003</v>
       </c>
+      <c r="C55" s="8"/>
+      <c r="D55" s="10"/>
     </row>
     <row r="56" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B56" s="11">
-        <v>45046</v>
-      </c>
-      <c r="C56" s="8" t="str">
-        <v>C</v>
-      </c>
-      <c r="D56" s="12">
         <v>0.22000000000000003</v>
       </c>
+      <c r="C56" s="8"/>
+      <c r="D56" s="12"/>
     </row>
     <row r="57" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B57" s="11">
-        <v>45077</v>
-      </c>
-      <c r="C57" s="8" t="str">
-        <v>C</v>
-      </c>
-      <c r="D57" s="10">
         <v>0.34</v>
       </c>
+      <c r="C57" s="8"/>
+      <c r="D57" s="10"/>
     </row>
     <row r="58" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B58" s="11">
-        <v>45107</v>
-      </c>
-      <c r="C58" s="8" t="str">
-        <v>C</v>
-      </c>
-      <c r="D58" s="12">
         <v>0.34</v>
       </c>
+      <c r="C58" s="8"/>
+      <c r="D58" s="12"/>
     </row>
     <row r="59" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B59" s="11">
-        <v>45138</v>
-      </c>
-      <c r="C59" s="8" t="str">
-        <v>C</v>
-      </c>
-      <c r="D59" s="10">
         <v>0.44</v>
       </c>
+      <c r="C59" s="8"/>
+      <c r="D59" s="10"/>
     </row>
     <row r="60" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B60" s="11">
-        <v>45169</v>
-      </c>
-      <c r="C60" s="8" t="str">
-        <v>C</v>
-      </c>
-      <c r="D60" s="12">
         <v>0.44</v>
       </c>
+      <c r="C60" s="8"/>
+      <c r="D60" s="12"/>
     </row>
     <row r="61" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B61" s="11">
-        <v>45199</v>
-      </c>
-      <c r="C61" s="8" t="str">
-        <v>C</v>
-      </c>
-      <c r="D61" s="10">
         <v>0.6</v>
       </c>
+      <c r="C61" s="8"/>
+      <c r="D61" s="10"/>
     </row>
     <row r="62" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B62" s="11">
-        <v>45230</v>
-      </c>
-      <c r="C62" s="8" t="str">
-        <v>C</v>
-      </c>
-      <c r="D62" s="12">
         <v>0.6</v>
       </c>
+      <c r="C62" s="8"/>
+      <c r="D62" s="12"/>
     </row>
     <row r="63" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B63" s="11">
-        <v>45260</v>
-      </c>
-      <c r="C63" s="8" t="str">
-        <v>C</v>
-      </c>
-      <c r="D63" s="10">
         <v>0.72</v>
       </c>
+      <c r="C63" s="8"/>
+      <c r="D63" s="10"/>
     </row>
     <row r="64" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B64" s="11">
-        <v>45291</v>
-      </c>
-      <c r="C64" s="8" t="str">
-        <v>C</v>
-      </c>
-      <c r="D64" s="10">
         <v>0.73</v>
       </c>
+      <c r="C64" s="8"/>
+      <c r="D64" s="10"/>
     </row>
     <row r="70" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B70" s="11" cm="1">
@@ -3557,4 +3471,1916 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E264AD69-428D-4857-9141-90CD86BE8638}">
+  <dimension ref="A5:S40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="8.796875" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:19" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>1</v>
+      </c>
+      <c r="B5" s="14">
+        <v>44957</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="F5" s="14" cm="1">
+        <f t="array" ref="F5:F40">_xlfn.LET(_xlpm.zz,_xlfn.REDUCE("",$A$5:$A$40,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,
+_xlfn.VSTACK(_xlpm.a,
+IF(ISNUMBER(INDEX($D$5:$D$40,_xlpm.v)),
+INDEX($D$5:$D$40,_xlpm.v),
+_xlfn.LET(
+_xlpm.nxt,_xlfn.TEXTBEFORE(_xlfn.TEXTJOIN(",",TRUE,INDEX($D$5:$D$40,_xlpm.v):$D$40),",")+0,
+_xlpm.off,_xlfn.XMATCH(_xlpm.nxt,INDEX($D$5:$D$40,_xlpm.v):$D$40,1),
+_xlpm.prev,_xlfn.TAKE(_xlpm.a,-1),(_xlpm.nxt-_xlpm.prev)/_xlpm.off+_xlpm.prev
+)
+)
+)
+)
+),
+_xlfn.DROP(_xlpm.zz,1))</f>
+        <v>0.05</v>
+      </c>
+      <c r="K5" s="14" t="b" cm="1">
+        <f t="array" ref="K5:K40">_xlfn.ANCHORARRAY(F5)=EDA!J3:J38</f>
+        <v>1</v>
+      </c>
+      <c r="M5" s="16" cm="1">
+        <f t="array" ref="M5:N22">_xlfn.LET(_xlpm.zz,_xlfn.REDUCE("",$A$5:$A$40,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,
+_xlfn.VSTACK(_xlpm.a,
+IF(ISNUMBER(INDEX($D$5:$D$40,_xlpm.v)),
+INDEX($D$5:$D$40,_xlpm.v),
+_xlfn.LET(
+_xlpm.nxt,_xlfn.TEXTBEFORE(_xlfn.TEXTJOIN(",",TRUE,INDEX($D$5:$D$40,_xlpm.v):$D$40),",")+0,
+_xlpm.off,_xlfn.XMATCH(_xlpm.nxt,INDEX($D$5:$D$40,_xlpm.v):$D$40,1),
+_xlpm.prev,_xlfn.TAKE(_xlpm.a,-1),(_xlpm.nxt-_xlpm.prev)/_xlpm.off+_xlpm.prev
+)
+)
+)
+)
+),
+_xlpm.mm, _xlfn.DROP(_xlpm.zz,1),
+_xlpm.xx, _xlfn.LET(
+_xlpm.c,_xlfn.UNIQUE(C3:C21),
+_xlpm.q,_xlfn.REDUCE("",_xlpm.c,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.LET(_xlpm.t,_xlfn._xlws.FILTER(B3:C21,C3:C21=_xlpm.v),_xlpm.mx,MAX(_xlfn.TAKE(_xlpm.t,,1)),_xlpm.mn,MIN(_xlfn.TAKE(_xlpm.t,,1)),_xlfn.VSTACK(_xlpm.a,_xlfn.LET(_xlpm.zz,_xlfn.UNIQUE(EOMONTH(_xlfn.SEQUENCE(_xlpm.mx-_xlpm.mn+1,1,_xlpm.mn),0)),_xlpm.yy,_xlfn.MAKEARRAY(LEN(_xlpm.zz),1,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,_xlpm.v)),_xlfn.HSTACK(_xlpm.zz,_xlpm.yy)))))),
+_xlpm._q,_xlfn.DROP(_xlpm.q,1),
+_xlpm.r,_xlfn.BYROW(_xlpm._q,_xlfn.LAMBDA(_xlpm.r,_xlfn.TEXTJOIN("",TRUE,_xlpm.r))),
+_xlpm.mm,_xlfn.XLOOKUP(_xlpm.r,B3:B21&amp;C3:C21,D3:D21,""),
+_xlpm.vv,_xlfn.DROP(_xlfn.REDUCE("",_xlpm.mm,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,IF(_xlpm.v="",_xlfn.TAKE(_xlpm.a,-1),_xlpm.v)))),1),
+_xlpm._q
+),_xlpm.xx
+)</f>
+        <v>31</v>
+      </c>
+      <c r="N5" s="14">
+        <v>0</v>
+      </c>
+      <c r="P5" s="14" cm="1">
+        <f t="array" aca="1" ref="P5:P40" ca="1">_xlfn.LET(_xlpm.zz,_xlfn.REDUCE("",$A$5:$A$40,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,
+_xlfn.VSTACK(_xlpm.a,
+IF(ISNUMBER(INDEX($D$5:$D$40,_xlpm.v)),
+INDEX($D$5:$D$40,_xlpm.v),
+_xlfn.LET(
+_xlpm.nxt,_xlfn.TEXTBEFORE(_xlfn.TEXTJOIN(",",TRUE,INDEX($D$5:$D$40,_xlpm.v):$D$40),",")+0,
+_xlpm.off,_xlfn.XMATCH(_xlpm.nxt,OFFSET($D$5:$D$40,_xlpm.v-1,0,36-_xlpm.v),1),
+_xlpm.prev,_xlfn.TAKE(_xlpm.a,-1),(_xlpm.nxt-_xlpm.prev)/_xlpm.off+_xlpm.prev
+)
+)
+)
+)
+),
+_xlfn.DROP(_xlpm.zz,1))</f>
+        <v>0.05</v>
+      </c>
+      <c r="S5" s="14" cm="1">
+        <f t="array" aca="1" ref="S5:S40" ca="1">_xlfn.LET(
+_xlpm.zz,_xlfn.REDUCE("",_xlfn.SEQUENCE(36),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,
+_xlfn.VSTACK(_xlpm.a,
+IF(ISNUMBER(INDEX($D$5:$D$40,_xlpm.v)),
+INDEX($D$5:$D$40,_xlpm.v),
+_xlfn.LET(
+_xlpm.nxt,_xlfn.TEXTBEFORE(_xlfn.TEXTJOIN(",",TRUE,INDEX($D$5:$D$40,_xlpm.v):$D$40),",")+0,
+_xlpm.off,_xlfn.XMATCH(_xlpm.nxt,OFFSET($D$5:$D$40,_xlpm.v-1,0,36-_xlpm.v),1),
+_xlpm.prev,_xlfn.TAKE(_xlpm.a,-1),(_xlpm.nxt-_xlpm.prev)/_xlpm.off+_xlpm.prev
+)
+)
+)
+)
+),
+_xlfn.DROP(_xlpm.zz,1))</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>2</v>
+      </c>
+      <c r="B6" s="14">
+        <v>44985</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F6" s="14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K6" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" s="14">
+        <v>44957</v>
+      </c>
+      <c r="N6" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="P6" s="14">
+        <f ca="1"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S6" s="14">
+        <f ca="1"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>3</v>
+      </c>
+      <c r="B7" s="14">
+        <v>45016</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="14">
+        <v>0.08</v>
+      </c>
+      <c r="F7" s="14">
+        <v>0.08</v>
+      </c>
+      <c r="K7" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" s="14">
+        <v>44985</v>
+      </c>
+      <c r="N7" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="P7" s="14">
+        <f ca="1"/>
+        <v>0.08</v>
+      </c>
+      <c r="S7" s="14">
+        <f ca="1"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>4</v>
+      </c>
+      <c r="B8" s="14">
+        <v>45046</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="14">
+        <v>0.12</v>
+      </c>
+      <c r="K8" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M8" s="14">
+        <v>45016</v>
+      </c>
+      <c r="N8" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="P8" s="14">
+        <f ca="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="S8" s="14">
+        <f ca="1"/>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>5</v>
+      </c>
+      <c r="B9" s="14">
+        <v>45077</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="14">
+        <v>0.16</v>
+      </c>
+      <c r="K9" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M9" s="14">
+        <v>45046</v>
+      </c>
+      <c r="N9" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="P9" s="14">
+        <f ca="1"/>
+        <v>0.16</v>
+      </c>
+      <c r="S9" s="14">
+        <f ca="1"/>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>6</v>
+      </c>
+      <c r="B10" s="14">
+        <v>45107</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="K10" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M10" s="14">
+        <v>45077</v>
+      </c>
+      <c r="N10" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="P10" s="14">
+        <f ca="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="S10" s="14">
+        <f ca="1"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>7</v>
+      </c>
+      <c r="B11" s="14">
+        <v>45138</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0.24</v>
+      </c>
+      <c r="F11" s="14">
+        <v>0.24</v>
+      </c>
+      <c r="K11" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M11" s="14">
+        <v>45107</v>
+      </c>
+      <c r="N11" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="P11" s="14">
+        <f ca="1"/>
+        <v>0.24</v>
+      </c>
+      <c r="S11" s="14">
+        <f ca="1"/>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>8</v>
+      </c>
+      <c r="B12" s="14">
+        <v>45169</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="K12" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M12" s="14">
+        <v>45138</v>
+      </c>
+      <c r="N12" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="P12" s="14">
+        <f ca="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="S12" s="14">
+        <f ca="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
+        <v>9</v>
+      </c>
+      <c r="B13" s="14">
+        <v>45199</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="14">
+        <v>0.26</v>
+      </c>
+      <c r="F13" s="14">
+        <v>0.26</v>
+      </c>
+      <c r="K13" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13" s="14">
+        <v>45169</v>
+      </c>
+      <c r="N13" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="P13" s="14">
+        <f ca="1"/>
+        <v>0.26</v>
+      </c>
+      <c r="S13" s="14">
+        <f ca="1"/>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>10</v>
+      </c>
+      <c r="B14" s="14">
+        <v>45230</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="14">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K14" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" s="14">
+        <v>45199</v>
+      </c>
+      <c r="N14" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="P14" s="14">
+        <f ca="1"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="S14" s="14">
+        <f ca="1"/>
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>11</v>
+      </c>
+      <c r="B15" s="14">
+        <v>45260</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="14">
+        <v>0.31999999999999995</v>
+      </c>
+      <c r="K15" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M15" s="14">
+        <v>45230</v>
+      </c>
+      <c r="N15" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="P15" s="14">
+        <f ca="1"/>
+        <v>0.31999999999999995</v>
+      </c>
+      <c r="S15" s="14">
+        <f ca="1"/>
+        <v>0.31999999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>12</v>
+      </c>
+      <c r="B16" s="14">
+        <v>45291</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="14">
+        <v>0.35</v>
+      </c>
+      <c r="F16" s="14">
+        <v>0.35</v>
+      </c>
+      <c r="K16" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M16" s="14">
+        <v>45260</v>
+      </c>
+      <c r="N16" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="P16" s="14">
+        <f ca="1"/>
+        <v>0.35</v>
+      </c>
+      <c r="S16" s="14">
+        <f ca="1"/>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>13</v>
+      </c>
+      <c r="B17" s="14">
+        <v>44957</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="F17" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="K17" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M17" s="14">
+        <v>45291</v>
+      </c>
+      <c r="N17" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="P17" s="14">
+        <f ca="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="S17" s="14">
+        <f ca="1"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>14</v>
+      </c>
+      <c r="B18" s="14">
+        <v>44985</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="14">
+        <v>0.04</v>
+      </c>
+      <c r="F18" s="14">
+        <v>0.04</v>
+      </c>
+      <c r="K18" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M18" s="14">
+        <v>44957</v>
+      </c>
+      <c r="N18" s="14" t="str">
+        <v>B</v>
+      </c>
+      <c r="P18" s="14">
+        <f ca="1"/>
+        <v>0.04</v>
+      </c>
+      <c r="S18" s="14">
+        <f ca="1"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <v>15</v>
+      </c>
+      <c r="B19" s="14">
+        <v>45016</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="14">
+        <v>0.08</v>
+      </c>
+      <c r="K19" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M19" s="14">
+        <v>44985</v>
+      </c>
+      <c r="N19" s="14" t="str">
+        <v>B</v>
+      </c>
+      <c r="P19" s="14">
+        <f ca="1"/>
+        <v>0.08</v>
+      </c>
+      <c r="S19" s="14">
+        <f ca="1"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <v>16</v>
+      </c>
+      <c r="B20" s="14">
+        <v>45046</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="14">
+        <v>0.12</v>
+      </c>
+      <c r="K20" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M20" s="14">
+        <v>45016</v>
+      </c>
+      <c r="N20" s="14" t="str">
+        <v>B</v>
+      </c>
+      <c r="P20" s="14">
+        <f ca="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="S20" s="14">
+        <f ca="1"/>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>17</v>
+      </c>
+      <c r="B21" s="14">
+        <v>45077</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="14">
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="F21" s="14">
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="K21" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M21" s="14">
+        <v>45046</v>
+      </c>
+      <c r="N21" s="14" t="str">
+        <v>B</v>
+      </c>
+      <c r="P21" s="14">
+        <f ca="1"/>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="S21" s="14">
+        <f ca="1"/>
+        <v>0.16000000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="14">
+        <v>18</v>
+      </c>
+      <c r="B22" s="14">
+        <v>45107</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="14">
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="F22" s="14">
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="K22" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M22" s="14">
+        <v>45077</v>
+      </c>
+      <c r="N22" s="14" t="str">
+        <v>B</v>
+      </c>
+      <c r="P22" s="14">
+        <f ca="1"/>
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="S22" s="14">
+        <f ca="1"/>
+        <v>0.21000000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
+        <v>19</v>
+      </c>
+      <c r="B23" s="14">
+        <v>45138</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="14">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="K23" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P23" s="14">
+        <f ca="1"/>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="S23" s="14">
+        <f ca="1"/>
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
+        <v>20</v>
+      </c>
+      <c r="B24" s="14">
+        <v>45169</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="14">
+        <v>0.24000000000000002</v>
+      </c>
+      <c r="F24" s="14">
+        <v>0.24000000000000002</v>
+      </c>
+      <c r="K24" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P24" s="14">
+        <f ca="1"/>
+        <v>0.24000000000000002</v>
+      </c>
+      <c r="S24" s="14">
+        <f ca="1"/>
+        <v>0.24000000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <v>21</v>
+      </c>
+      <c r="B25" s="14">
+        <v>45199</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="14">
+        <v>0.29000000000000004</v>
+      </c>
+      <c r="K25" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P25" s="14">
+        <f ca="1"/>
+        <v>0.29000000000000004</v>
+      </c>
+      <c r="S25" s="14">
+        <f ca="1"/>
+        <v>0.29000000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
+        <v>22</v>
+      </c>
+      <c r="B26" s="14">
+        <v>45230</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="K26" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P26" s="14">
+        <f ca="1"/>
+        <v>0.34</v>
+      </c>
+      <c r="S26" s="14">
+        <f ca="1"/>
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <v>23</v>
+      </c>
+      <c r="B27" s="14">
+        <v>45260</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="14">
+        <v>0.39</v>
+      </c>
+      <c r="K27" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P27" s="14">
+        <f ca="1"/>
+        <v>0.39</v>
+      </c>
+      <c r="S27" s="14">
+        <f ca="1"/>
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <v>24</v>
+      </c>
+      <c r="B28" s="14">
+        <v>45291</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="14">
+        <v>0.44</v>
+      </c>
+      <c r="F28" s="14">
+        <v>0.44</v>
+      </c>
+      <c r="K28" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P28" s="14">
+        <f ca="1"/>
+        <v>0.44</v>
+      </c>
+      <c r="S28" s="14">
+        <f ca="1"/>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>25</v>
+      </c>
+      <c r="B29" s="14">
+        <v>44957</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F29" s="14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K29" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P29" s="14">
+        <f ca="1"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S29" s="14">
+        <f ca="1"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
+        <v>26</v>
+      </c>
+      <c r="B30" s="14">
+        <v>44985</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="14">
+        <v>0.14500000000000002</v>
+      </c>
+      <c r="K30" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P30" s="14">
+        <f ca="1"/>
+        <v>0.14500000000000002</v>
+      </c>
+      <c r="S30" s="14">
+        <f ca="1"/>
+        <v>0.14500000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
+        <v>27</v>
+      </c>
+      <c r="B31" s="14">
+        <v>45016</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="14">
+        <v>0.22000000000000003</v>
+      </c>
+      <c r="F31" s="14">
+        <v>0.22000000000000003</v>
+      </c>
+      <c r="K31" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P31" s="14">
+        <f ca="1"/>
+        <v>0.22000000000000003</v>
+      </c>
+      <c r="S31" s="14">
+        <f ca="1"/>
+        <v>0.22000000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>28</v>
+      </c>
+      <c r="B32" s="14">
+        <v>45046</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="14">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K32" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P32" s="14">
+        <f ca="1"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="S32" s="14">
+        <f ca="1"/>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>29</v>
+      </c>
+      <c r="B33" s="14">
+        <v>45077</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="F33" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="K33" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P33" s="14">
+        <f ca="1"/>
+        <v>0.34</v>
+      </c>
+      <c r="S33" s="14">
+        <f ca="1"/>
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
+        <v>30</v>
+      </c>
+      <c r="B34" s="14">
+        <v>45107</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="14">
+        <v>0.39</v>
+      </c>
+      <c r="K34" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P34" s="14">
+        <f ca="1"/>
+        <v>0.39</v>
+      </c>
+      <c r="S34" s="14">
+        <f ca="1"/>
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" s="14">
+        <v>31</v>
+      </c>
+      <c r="B35" s="14">
+        <v>45138</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="14">
+        <v>0.44</v>
+      </c>
+      <c r="F35" s="14">
+        <v>0.44</v>
+      </c>
+      <c r="K35" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P35" s="14">
+        <f ca="1"/>
+        <v>0.44</v>
+      </c>
+      <c r="S35" s="14">
+        <f ca="1"/>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
+        <v>32</v>
+      </c>
+      <c r="B36" s="14">
+        <v>45169</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="14">
+        <v>0.52</v>
+      </c>
+      <c r="K36" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P36" s="14">
+        <f ca="1"/>
+        <v>0.52</v>
+      </c>
+      <c r="S36" s="14">
+        <f ca="1"/>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="14">
+        <v>33</v>
+      </c>
+      <c r="B37" s="14">
+        <v>45199</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="F37" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="K37" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P37" s="14">
+        <f ca="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="S37" s="14">
+        <f ca="1"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" s="14">
+        <v>34</v>
+      </c>
+      <c r="B38" s="14">
+        <v>45230</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="14">
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="K38" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P38" s="14">
+        <f ca="1"/>
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="S38" s="14">
+        <f ca="1"/>
+        <v>0.65999999999999992</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" s="14">
+        <v>35</v>
+      </c>
+      <c r="B39" s="14">
+        <v>45260</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="14">
+        <v>0.72</v>
+      </c>
+      <c r="F39" s="14">
+        <v>0.72</v>
+      </c>
+      <c r="K39" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P39" s="14">
+        <f ca="1"/>
+        <v>0.72</v>
+      </c>
+      <c r="S39" s="14">
+        <f ca="1"/>
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40" s="14">
+        <v>36</v>
+      </c>
+      <c r="B40" s="14">
+        <v>45291</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="14">
+        <v>0.73</v>
+      </c>
+      <c r="F40" s="14">
+        <v>0.73</v>
+      </c>
+      <c r="K40" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P40" s="14">
+        <f ca="1"/>
+        <v>0.73</v>
+      </c>
+      <c r="S40" s="14">
+        <f ca="1"/>
+        <v>0.73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1934A1-FE57-414E-97C2-D14287DFED05}">
+  <dimension ref="A1:U38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="2" max="3" width="12.3984375" customWidth="1"/>
+    <col min="4" max="4" width="13.19921875" customWidth="1"/>
+    <col min="5" max="5" width="15.3984375" customWidth="1"/>
+    <col min="6" max="6" width="38.59765625" customWidth="1"/>
+    <col min="7" max="7" width="8.3984375" customWidth="1"/>
+    <col min="8" max="8" width="15.3984375" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="10" max="10" width="13.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+    </row>
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="11">
+        <v>44957</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="H3" s="11">
+        <v>44957</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="10">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="11">
+        <v>44985</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H4" s="11">
+        <v>44985</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="11">
+        <v>45016</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.08</v>
+      </c>
+      <c r="H5" s="11">
+        <v>45016</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="11">
+        <v>45138</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.24</v>
+      </c>
+      <c r="H6" s="11">
+        <v>45046</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="12">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="11">
+        <v>45199</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.26</v>
+      </c>
+      <c r="H7" s="11">
+        <v>45077</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="12">
+        <v>0.15999999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="11">
+        <v>45291</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.35</v>
+      </c>
+      <c r="F8"/>
+      <c r="H8" s="11">
+        <v>45107</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="12">
+        <v>0.19999999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="11">
+        <v>44957</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="H9" s="11">
+        <v>45138</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="10">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="11">
+        <v>44985</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="H10" s="11">
+        <v>45169</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="12">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="11">
+        <v>45077</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="H11" s="11">
+        <v>45199</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0.26</v>
+      </c>
+      <c r="S11"/>
+      <c r="T11"/>
+      <c r="U11"/>
+    </row>
+    <row r="12" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="11">
+        <v>45107</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="11">
+        <v>45230</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="11">
+        <v>45169</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.24000000000000002</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="11">
+        <v>45260</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="12">
+        <v>0.31999999999999995</v>
+      </c>
+      <c r="R13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="11">
+        <v>45291</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0.44</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="H14" s="11">
+        <v>45291</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="10">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="11">
+        <v>44957</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H15" s="11">
+        <v>44957</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" s="10">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="11">
+        <v>45016</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0.22000000000000003</v>
+      </c>
+      <c r="H16" s="11">
+        <v>44985</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" s="10">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="11">
+        <v>45077</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0.34</v>
+      </c>
+      <c r="H17" s="11">
+        <v>45016</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" s="12">
+        <v>8.0000000000000016E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="11">
+        <v>45138</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0.44</v>
+      </c>
+      <c r="H18" s="11">
+        <v>45046</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J18" s="12">
+        <v>0.12000000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="11">
+        <v>45199</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="H19" s="11">
+        <v>45077</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J19" s="10">
+        <v>0.16000000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="11">
+        <v>45260</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0.72</v>
+      </c>
+      <c r="H20" s="11">
+        <v>45107</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J20" s="10">
+        <v>0.21000000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="11">
+        <v>45291</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0.73</v>
+      </c>
+      <c r="H21" s="11">
+        <v>45138</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J21" s="12">
+        <v>0.22500000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="H22" s="11">
+        <v>45169</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J22" s="10">
+        <v>0.24000000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="H23" s="11">
+        <v>45199</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J23" s="12">
+        <v>0.29000000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
+      <c r="H24" s="11">
+        <v>45230</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J24" s="12">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" t="e" cm="1">
+        <f t="array" aca="1" ref="B25" ca="1">_xlfn.LET(
+_xlpm.nn,_xlfn.LET(
+_xlpm.c,_xlfn.UNIQUE(C3:C21),
+_xlpm.q,_xlfn.REDUCE("",_xlpm.c,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.LET(_xlpm.t,_xlfn._xlws.FILTER(B3:C21,C3:C21=_xlpm.v),_xlpm.mx,MAX(_xlfn.TAKE(_xlpm.t,,1)),_xlpm.mn,MIN(_xlfn.TAKE(_xlpm.t,,1)),_xlfn.VSTACK(_xlpm.a,_xlfn.LET(_xlpm.zz,_xlfn.UNIQUE(EOMONTH(_xlfn.SEQUENCE(_xlpm.mx-_xlpm.mn+1,1,_xlpm.mn),0)),_xlpm.yy,_xlfn.MAKEARRAY(LEN(_xlpm.zz),1,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,_xlpm.v)),_xlfn.HSTACK(_xlpm.zz,_xlpm.yy)))))),
+_xlpm._q,_xlfn.DROP(_xlpm.q,1),
+_xlpm.r,_xlfn.BYROW(_xlpm._q,_xlfn.LAMBDA(_xlpm.r,_xlfn.TEXTJOIN("",TRUE,_xlpm.r))),
+_xlpm.mm,_xlfn.XLOOKUP(_xlpm.r,B3:B21&amp;C3:C21,D3:D21,""),
+_xlfn.HSTACK(_xlpm._q,_xlpm.mm)
+),
+_xlpm.cc,_xlfn.LET(_xlpm.ff,_xlfn.LET(
+_xlpm.c,_xlfn.UNIQUE(C3:C21),
+_xlpm.q,_xlfn.REDUCE("",_xlpm.c,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.LET(_xlpm.t,_xlfn._xlws.FILTER(B3:C21,C3:C21=_xlpm.v),_xlpm.mx,MAX(_xlfn.TAKE(_xlpm.t,,1)),_xlpm.mn,MIN(_xlfn.TAKE(_xlpm.t,,1)),_xlfn.VSTACK(_xlpm.a,_xlfn.LET(_xlpm.zz,_xlfn.UNIQUE(EOMONTH(_xlfn.SEQUENCE(_xlpm.mx-_xlpm.mn+1,1,_xlpm.mn),0)),_xlpm.yy,_xlfn.MAKEARRAY(LEN(_xlpm.zz),1,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,_xlpm.v)),_xlfn.HSTACK(_xlpm.zz,_xlpm.yy)))))),
+_xlpm._q,_xlfn.DROP(_xlpm.q,1),
+_xlpm.r,_xlfn.BYROW(_xlpm._q,_xlfn.LAMBDA(_xlpm.r,_xlfn.TEXTJOIN("",TRUE,_xlpm.r))),
+_xlpm.mm,_xlfn.XLOOKUP(_xlpm.r,B3:B21&amp;C3:C21,D3:D21,""),
+_xlfn.HSTACK(_xlpm._q,_xlpm.mm)
+),_xlpm.ff),
+_xlpm.ee,_xlfn.LET(_xlpm.zz,_xlfn.REDUCE("",_xlfn.SEQUENCE(36-v,1,v),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,
+_xlfn.VSTACK(_xlpm.a,
+IF(ISNUMBER(INDEX(_xlfn.TAKE(_xlpm.nn,-1),_xlpm.v)),
+INDEX(_xlfn.TAKE(_xlpm.nn,-1),_xlpm.v),
+_xlfn.LET(
+_xlpm.nxt,_xlfn.TEXTBEFORE(_xlfn.TEXTJOIN(",",TRUE,INDEX(_xlfn.TAKE(_xlpm.nn,-1),_xlpm.v)),",")+0,
+_xlpm.off,_xlfn.XMATCH(_xlpm.nxt,OFFSET(_xlfn.TAKE(_xlpm.nn,-1),_xlpm.v-1,0,36-_xlpm.v),1),
+_xlpm.prev,_xlfn.TAKE(_xlpm.a,-1),(_xlpm.nxt-_xlpm.prev)/_xlpm.off+_xlpm.prev
+)
+)
+)
+)
+),
+_xlfn.DROP(_xlpm.zz,1)),_xlpm.ee
+)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H25" s="11">
+        <v>45260</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J25" s="12">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="H26" s="11">
+        <v>45291</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J26" s="10">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="H27" s="11">
+        <v>44957</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J27" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="H28" s="11">
+        <v>44985</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J28" s="12">
+        <v>0.14500000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
+      <c r="H29" s="11">
+        <v>45016</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J29" s="10">
+        <v>0.22000000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+      <c r="H30" s="11">
+        <v>45046</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J30" s="12">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="5"/>
+      <c r="H31" s="11">
+        <v>45077</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J31" s="10">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H32" s="11">
+        <v>45107</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J32" s="12">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+      <c r="H33" s="11">
+        <v>45138</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J33" s="10">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H34" s="11">
+        <v>45169</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J34" s="12">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="5"/>
+      <c r="H35" s="11">
+        <v>45199</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J35" s="10">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="5"/>
+      <c r="H36" s="11">
+        <v>45230</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36" s="12">
+        <v>0.65999999999999992</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="5"/>
+      <c r="H37" s="11">
+        <v>45260</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37" s="10">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="5"/>
+      <c r="H38" s="11">
+        <v>45291</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J38" s="10">
+        <v>0.73</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="H1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>